<commit_message>
Cleaned up diversity analysis section and dataframes:
</commit_message>
<xml_diff>
--- a/Data/Sequencing_run/GSF3417-Lennon-McMullen-Summary.xlsx
+++ b/Data/Sequencing_run/GSF3417-Lennon-McMullen-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmcmullen/GitHub/rhizo.rb.tnseq/Data/Sequencing_run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5D767C5-ED7B-8E4F-B7A7-087175A23FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22127D2-15BF-AE44-B33F-8C42A9BAC5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{225CD9E5-7643-4BE6-BBDA-3D4BE40A4650}"/>
+    <workbookView xWindow="10320" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{225CD9E5-7643-4BE6-BBDA-3D4BE40A4650}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,12 +478,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="28">
@@ -883,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1002,11 +1008,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1318,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A975F75-0941-4A8B-9ABF-BD2B7D2AB5D5}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1808,7 +1828,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="42" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -1840,7 +1860,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="14" t="s">
@@ -1872,7 +1892,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -1904,7 +1924,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="42" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -1968,7 +1988,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="14" t="s">
@@ -2000,7 +2020,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="42" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="14" t="s">
@@ -2032,7 +2052,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="42" t="s">
         <v>61</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -2064,7 +2084,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="42" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="14" t="s">
@@ -2128,7 +2148,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="42" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="14" t="s">
@@ -2160,7 +2180,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="42" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -2192,7 +2212,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="42" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -2224,7 +2244,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="42" t="s">
         <v>73</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -2288,7 +2308,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="42" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="14" t="s">
@@ -2352,7 +2372,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="42" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -2416,7 +2436,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="42" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -2480,7 +2500,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="42" t="s">
         <v>89</v>
       </c>
       <c r="B46" s="14" t="s">
@@ -2512,7 +2532,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="42" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -2544,7 +2564,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="42" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -2576,7 +2596,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="42" t="s">
         <v>95</v>
       </c>
       <c r="B49" s="14" t="s">
@@ -2608,7 +2628,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="42" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -2640,7 +2660,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="42" t="s">
         <v>99</v>
       </c>
       <c r="B51" s="14" t="s">
@@ -3076,6 +3096,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A72:A82"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -3084,8 +3105,12 @@
     <mergeCell ref="B62:B63"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="G62:G63"/>
-    <mergeCell ref="A72:A82"/>
   </mergeCells>
+  <conditionalFormatting sqref="C13:C57">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>500000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>